<commit_message>
changed up order and naming of scripts
</commit_message>
<xml_diff>
--- a/data_in/CropData/McHenry_Crop_Acres.xlsx
+++ b/data_in/CropData/McHenry_Crop_Acres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/paulukonis_elizabeth_epa_gov/Documents/Profile/Documents/GitHub/pollinator_probabilistic_loading/data_in/CropData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="8_{D8131C6C-C8FD-4B4C-929E-AA606F2FC4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2A64E0D-35D2-4AF6-920D-D9E40B80830E}"/>
+  <xr:revisionPtr revIDLastSave="120" documentId="8_{D8131C6C-C8FD-4B4C-929E-AA606F2FC4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9B40D4D-1B9D-42FE-8E70-2DAA84A92836}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{9816FF81-C81C-4D19-88AD-9676C023C497}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9816FF81-C81C-4D19-88AD-9676C023C497}"/>
   </bookViews>
   <sheets>
     <sheet name="CoA" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="52">
   <si>
     <t>Program</t>
   </si>
@@ -165,6 +165,36 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Mean By Crop</t>
+  </si>
+  <si>
+    <t>Mean By Year</t>
+  </si>
+  <si>
+    <t>Difference from Analysis (i.e., percent difference in total estimated crop area)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total crop footprint comparison </t>
+  </si>
+  <si>
+    <t>subfield could never be NA</t>
+  </si>
+  <si>
+    <t>1- NA comparison</t>
+  </si>
+  <si>
+    <t>Pesticide vs. nonpesticide</t>
+  </si>
+  <si>
+    <t>Subtract fields from NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get TOTAL area, and substract Nas from that, and compare to the area of the fields in the delineation layer </t>
+  </si>
+  <si>
+    <t>How</t>
   </si>
 </sst>
 </file>
@@ -525,23 +555,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF545BB8-BADE-42A8-BBA6-7BDE1CEB1F8A}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:V15"/>
+  <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD15"/>
+    <sheetView tabSelected="1" topLeftCell="J10" workbookViewId="0">
+      <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="16" max="16" width="22.7265625" customWidth="1"/>
-    <col min="17" max="17" width="40.1796875" customWidth="1"/>
+    <col min="16" max="16" width="16.90625" customWidth="1"/>
+    <col min="17" max="17" width="14.7265625" customWidth="1"/>
     <col min="18" max="18" width="10.08984375" customWidth="1"/>
     <col min="19" max="19" width="15.7265625" customWidth="1"/>
     <col min="20" max="20" width="6.6328125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -606,15 +636,21 @@
         <v>20</v>
       </c>
       <c r="V1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+      <c r="W1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>21</v>
       </c>
       <c r="B2">
-        <v>2017</v>
+        <v>1997</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
@@ -656,18 +692,19 @@
         <v>30</v>
       </c>
       <c r="T2" s="3">
-        <v>92962</v>
-      </c>
-      <c r="U2">
-        <v>13.4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+        <v>103822</v>
+      </c>
+      <c r="V2">
+        <f>AVERAGE(T1:T2)</f>
+        <v>103822</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
       <c r="B3">
-        <v>2012</v>
+        <v>1997</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -697,10 +734,10 @@
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="R3" t="s">
         <v>29</v>
@@ -709,18 +746,30 @@
         <v>30</v>
       </c>
       <c r="T3" s="3">
-        <v>123654</v>
-      </c>
-      <c r="U3">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+        <v>73566</v>
+      </c>
+      <c r="V3">
+        <f>AVERAGE(T1:T3)</f>
+        <v>88694</v>
+      </c>
+      <c r="W3">
+        <f>SUM(T2:T3)</f>
+        <v>177388</v>
+      </c>
+      <c r="X3">
+        <f>(Y3-W3)/W3</f>
+        <v>-0.17418934764471106</v>
+      </c>
+      <c r="Y3">
+        <v>146488.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
       <c r="B4">
-        <v>2007</v>
+        <v>2002</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -762,10 +811,10 @@
         <v>30</v>
       </c>
       <c r="T4" s="3">
-        <v>121403</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+        <v>96978</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -800,10 +849,10 @@
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="Q5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="R5" t="s">
         <v>29</v>
@@ -812,15 +861,15 @@
         <v>30</v>
       </c>
       <c r="T5" s="3">
-        <v>96978</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+        <v>77340</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
       <c r="B6">
-        <v>1997</v>
+        <v>2002</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -850,10 +899,10 @@
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="Q6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="R6" t="s">
         <v>29</v>
@@ -862,19 +911,27 @@
         <v>30</v>
       </c>
       <c r="T6" s="3">
-        <v>103822</v>
+        <v>3396</v>
       </c>
       <c r="V6">
-        <f>AVERAGE(T2:T6)</f>
-        <v>107763.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+        <f>AVERAGE(T3:T6)</f>
+        <v>62820</v>
+      </c>
+      <c r="W6">
+        <f>SUM(T4:T6)</f>
+        <v>177714</v>
+      </c>
+      <c r="X6">
+        <f>(Y3-W6)/W6</f>
+        <v>-0.17570422138942349</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>21</v>
       </c>
       <c r="B7">
-        <v>2017</v>
+        <v>2007</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
@@ -904,10 +961,10 @@
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R7" t="s">
         <v>29</v>
@@ -916,18 +973,15 @@
         <v>30</v>
       </c>
       <c r="T7" s="3">
-        <v>67086</v>
-      </c>
-      <c r="U7">
-        <v>14.6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+        <v>121403</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>21</v>
       </c>
       <c r="B8">
-        <v>2012</v>
+        <v>2007</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
@@ -969,13 +1023,10 @@
         <v>30</v>
       </c>
       <c r="T8" s="3">
-        <v>58099</v>
-      </c>
-      <c r="U8">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+        <v>41823</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1010,10 +1061,10 @@
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="Q9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R9" t="s">
         <v>29</v>
@@ -1022,15 +1073,23 @@
         <v>30</v>
       </c>
       <c r="T9" s="3">
-        <v>41823</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+        <v>7658</v>
+      </c>
+      <c r="W9">
+        <f>SUM(T7:T9)</f>
+        <v>170884</v>
+      </c>
+      <c r="X9">
+        <f>(Y3-W9)/W9</f>
+        <v>-0.14275824535942513</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>21</v>
       </c>
       <c r="B10">
-        <v>2002</v>
+        <v>2012</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
@@ -1060,10 +1119,10 @@
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="R10" t="s">
         <v>29</v>
@@ -1072,15 +1131,18 @@
         <v>30</v>
       </c>
       <c r="T10" s="3">
-        <v>77340</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+        <v>123654</v>
+      </c>
+      <c r="U10">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>21</v>
       </c>
       <c r="B11">
-        <v>1997</v>
+        <v>2012</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
@@ -1122,19 +1184,18 @@
         <v>30</v>
       </c>
       <c r="T11" s="3">
-        <v>73566</v>
-      </c>
-      <c r="V11">
-        <f>AVERAGE(T7:T11)</f>
-        <v>63582.8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+        <v>58099</v>
+      </c>
+      <c r="U11">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>21</v>
       </c>
       <c r="B12">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="C12" t="s">
         <v>22</v>
@@ -1176,18 +1237,26 @@
         <v>30</v>
       </c>
       <c r="T12" s="3">
-        <v>2910</v>
+        <v>3684</v>
       </c>
       <c r="U12">
-        <v>26.4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+        <v>6.1</v>
+      </c>
+      <c r="W12">
+        <f>SUM(T10:T12)</f>
+        <v>185437</v>
+      </c>
+      <c r="X12">
+        <f>(Y3-W12)/W12</f>
+        <v>-0.21003413558243503</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>21</v>
       </c>
       <c r="B13">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="C13" t="s">
         <v>22</v>
@@ -1217,10 +1286,10 @@
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="Q13" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="R13" t="s">
         <v>29</v>
@@ -1229,18 +1298,18 @@
         <v>30</v>
       </c>
       <c r="T13" s="3">
-        <v>3684</v>
+        <v>92962</v>
       </c>
       <c r="U13">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>21</v>
       </c>
       <c r="B14">
-        <v>2007</v>
+        <v>2017</v>
       </c>
       <c r="C14" t="s">
         <v>22</v>
@@ -1270,10 +1339,10 @@
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="R14" t="s">
         <v>29</v>
@@ -1282,15 +1351,18 @@
         <v>30</v>
       </c>
       <c r="T14" s="3">
-        <v>7658</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+        <v>67086</v>
+      </c>
+      <c r="U14">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>21</v>
       </c>
       <c r="B15">
-        <v>2002</v>
+        <v>2017</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
@@ -1332,23 +1404,58 @@
         <v>30</v>
       </c>
       <c r="T15" s="3">
-        <v>3396</v>
-      </c>
-      <c r="V15">
-        <f>AVERAGE(T12:T15)</f>
-        <v>4412</v>
+        <v>2910</v>
+      </c>
+      <c r="U15">
+        <v>26.4</v>
+      </c>
+      <c r="W15">
+        <f>SUM(T13:T15)</f>
+        <v>162958</v>
+      </c>
+      <c r="X15">
+        <f>(Y3-W15)/W15</f>
+        <v>-0.10106346420550084</v>
+      </c>
+    </row>
+    <row r="19" spans="19:22" x14ac:dyDescent="0.35">
+      <c r="S19" t="s">
+        <v>47</v>
+      </c>
+      <c r="V19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="19:22" x14ac:dyDescent="0.35">
+      <c r="S20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="19:22" x14ac:dyDescent="0.35">
+      <c r="S22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="19:22" x14ac:dyDescent="0.35">
+      <c r="S25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="19:22" x14ac:dyDescent="0.35">
+      <c r="S26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="19:22" x14ac:dyDescent="0.35">
+      <c r="S29" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V15" xr:uid="{BF545BB8-BADE-42A8-BBA6-7BDE1CEB1F8A}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="1997"/>
-        <filter val="2002"/>
-        <filter val="2007"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:V15" xr:uid="{BF545BB8-BADE-42A8-BBA6-7BDE1CEB1F8A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W15">
+    <sortCondition ref="B1:B15"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4554,7 +4661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61049B34-FBC7-4179-AD7B-BB954EEB7163}">
   <dimension ref="B1:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G24" sqref="G24:G26"/>
     </sheetView>
   </sheetViews>
@@ -5001,7 +5108,7 @@
         <v>97858.25</v>
       </c>
       <c r="G24">
-        <f t="shared" ref="G23:G26" si="0">E24/F24</f>
+        <f t="shared" ref="G24:G26" si="0">E24/F24</f>
         <v>1.24060056254838</v>
       </c>
     </row>

</xml_diff>